<commit_message>
2commit (added comparision variabes)
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -353,10 +353,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0.2721761447142857</v>
+        <v>0.7947224918333333</v>
       </c>
       <c r="B2">
-        <v>0.2261217135714286</v>
+        <v>0.4174212148333334</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -369,10 +369,10 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.7947224918333333</v>
+        <v>0.2721761447142857</v>
       </c>
       <c r="B4">
-        <v>0.4174212148333334</v>
+        <v>0.2261217135714286</v>
       </c>
     </row>
     <row r="5" spans="1:2">

</xml_diff>

<commit_message>
15April commit with both csv and xlsx
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -353,31 +353,31 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>0.3940568957142857</v>
+        <v>0.8121888540000001</v>
       </c>
       <c r="B2">
-        <v>0.1618493064285715</v>
+        <v>0.2739612258</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>0.5338261285</v>
+        <v>0.2138739478333333</v>
       </c>
       <c r="B3">
-        <v>0.800905125</v>
+        <v>0.2538263863333334</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>0.6295969563999999</v>
+        <v>0.537878838</v>
       </c>
       <c r="B4">
-        <v>0.4466525456</v>
+        <v>0.7541248822857144</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -390,7 +390,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>0.348265448</v>
@@ -401,7 +401,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>0.234727223</v>
@@ -412,7 +412,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>0.7671849120000001</v>
@@ -423,7 +423,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>0.7166711099999999</v>
@@ -434,7 +434,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>0.919303164</v>
@@ -445,7 +445,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12">
         <v>0.344657111</v>
@@ -456,7 +456,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>0.456945687</v>
@@ -467,7 +467,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14">
         <v>0.276023884</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16">
         <v>0.235105096</v>
@@ -511,7 +511,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18">
         <v>0.5632956139999999</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B19">
         <v>0.464132225</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B20">
         <v>0.781520654</v>
@@ -544,7 +544,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21">
         <v>0.029144362</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B22">
         <v>0.834918083</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23">
         <v>0.050047786</v>

</xml_diff>